<commit_message>
ready to push to main
</commit_message>
<xml_diff>
--- a/Data/zcb value hedge.xlsx
+++ b/Data/zcb value hedge.xlsx
@@ -364,7 +364,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>189972.6342060384</v>
+        <v>-27872.73217226321</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -372,7 +372,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>482388.7191872528</v>
+        <v>-28505.19157816322</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -380,7 +380,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-387898.3602988338</v>
+        <v>-28951.16391042173</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -388,7 +388,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-521686.9224756696</v>
+        <v>-29322.46222077663</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -396,7 +396,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-24114.58100197818</v>
+        <v>-29465.67670647293</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -404,7 +404,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-108671.7521613445</v>
+        <v>-29270.15557835265</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -412,7 +412,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>236129.9554903601</v>
+        <v>-29085.13773181424</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -420,7 +420,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>84217.74204762869</v>
+        <v>-28919.83322262217</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -428,7 +428,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>-411730.673779253</v>
+        <v>-28608.05240017437</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -436,7 +436,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>-193965.2827945087</v>
+        <v>-28150.93408682003</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -444,7 +444,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>335393.9776508267</v>
+        <v>-27664.48673328008</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -452,7 +452,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>303091.2830366261</v>
+        <v>-27253.25510337381</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -460,7 +460,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>-226879.7080608735</v>
+        <v>-26723.8192678688</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -468,7 +468,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>-708799.0335552499</v>
+        <v>-26245.77455861241</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -476,7 +476,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>117140.2853844859</v>
+        <v>-25256.98877275228</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -484,7 +484,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>346311.2411510285</v>
+        <v>-24305.70329757581</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -492,7 +492,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>-109644.0946976269</v>
+        <v>-23973.6899340907</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -500,7 +500,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>-41537.71882348154</v>
+        <v>-23287.3223833589</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -508,7 +508,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>48908.73685001845</v>
+        <v>-22683.44833445781</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -516,7 +516,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>187025.7592545259</v>
+        <v>-22051.95055150932</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -524,7 +524,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>117285.5033899051</v>
+        <v>-21393.72180435376</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -532,7 +532,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>-329022.9142926881</v>
+        <v>-20714.1215496283</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -540,7 +540,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>61498.48472428961</v>
+        <v>-20140.64076975684</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -548,7 +548,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>112768.5970478198</v>
+        <v>-126522.0942230288</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -556,7 +556,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>-559363.0100845356</v>
+        <v>-15966.05072521717</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -564,7 +564,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>463670.1794426862</v>
+        <v>-15773.91933315351</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -572,7 +572,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>-78788.45640915415</v>
+        <v>-15472.58800625017</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -580,7 +580,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>294348.3372802587</v>
+        <v>-14941.39418334994</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -588,7 +588,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>95278.38435272602</v>
+        <v>-14709.02088501978</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -596,7 +596,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>-647948.6966344451</v>
+        <v>-14253.40069303035</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -604,7 +604,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>108783.530084362</v>
+        <v>-13963.84161733983</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -612,7 +612,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>-98372.86047954431</v>
+        <v>-13485.23445993945</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -620,7 +620,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>15775.84756581151</v>
+        <v>-13194.01049688353</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -628,7 +628,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>114405.229127757</v>
+        <v>-12842.43416880642</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -636,7 +636,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>-327766.9822421441</v>
+        <v>-12468.07131298199</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -644,7 +644,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>187784.5450846228</v>
+        <v>-118230.1708920357</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -652,7 +652,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>340700.8862185065</v>
+        <v>-10061.68160939902</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -660,7 +660,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>-254392.37628578</v>
+        <v>-9770.351655640088</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -668,7 +668,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>-472620.6173477172</v>
+        <v>-9576.845055425692</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -676,7 +676,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>142369.9131491241</v>
+        <v>-9399.691138934173</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -684,7 +684,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>543552.2483347143</v>
+        <v>-9482.200229550292</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -692,7 +692,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>219794.6342794911</v>
+        <v>-9179.840758572129</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -700,7 +700,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>168205.4759132406</v>
+        <v>-8818.489126861503</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -708,7 +708,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>-312889.0696984928</v>
+        <v>-8740.290892814754</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -716,7 +716,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>-949997.6848549069</v>
+        <v>-8532.524324760823</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -724,7 +724,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>666037.6817219502</v>
+        <v>-8435.810227489135</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -732,7 +732,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>159823.2114281049</v>
+        <v>-8287.447494908836</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -740,7 +740,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>-318190.4578006056</v>
+        <v>-8084.70816677213</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -748,7 +748,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>-57437.47476672564</v>
+        <v>-7858.009488631932</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -756,7 +756,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>197404.658200126</v>
+        <v>-7698.608058461469</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -764,7 +764,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>380889.8265051046</v>
+        <v>-7626.789900368242</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -772,7 +772,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>-526857.5558825018</v>
+        <v>-7421.600177721641</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -780,7 +780,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>-853353.0084345979</v>
+        <v>-7354.08262542528</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -788,7 +788,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>345724.1786111341</v>
+        <v>-7208.394319977569</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -796,7 +796,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>788771.4022960509</v>
+        <v>-7004.423362970527</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -804,7 +804,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>341749.3249959552</v>
+        <v>-6796.853457025359</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -812,7 +812,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>-463561.0260238043</v>
+        <v>-6689.817791154689</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -820,7 +820,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>-510461.0299742363</v>
+        <v>-6576.90674109983</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -828,7 +828,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>-449515.8191010049</v>
+        <v>-6471.391111436718</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -836,7 +836,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>153820.2892663355</v>
+        <v>-375344.5150015376</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -844,7 +844,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>309754.0593474839</v>
+        <v>-2501.172781160858</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -852,7 +852,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>-424959.4062204091</v>
+        <v>-2472.357800316604</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -860,7 +860,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>286483.6904868659</v>
+        <v>-2426.488532461176</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -868,7 +868,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>731613.3482321933</v>
+        <v>-2385.089875361895</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -876,7 +876,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>-252269.1719766216</v>
+        <v>-2342.260552554153</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -884,7 +884,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>-371507.8228738582</v>
+        <v>-2273.622500472011</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -892,7 +892,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>-195304.2796490671</v>
+        <v>-2246.925960998009</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -900,7 +900,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>314528.0836655751</v>
+        <v>-2180.457705455039</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -908,7 +908,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>-64033.46508429869</v>
+        <v>-2171.495254655041</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -916,7 +916,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>-398676.0392043573</v>
+        <v>-2121.71188378467</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -924,7 +924,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>546612.2329205499</v>
+        <v>-2113.768735606039</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -932,7 +932,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>430518.6061303429</v>
+        <v>-2082.956201836494</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -940,7 +940,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>-425065.2919919259</v>
+        <v>-2016.789928209417</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -948,7 +948,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>-6240.251027587311</v>
+        <v>-2016.834970768178</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -956,7 +956,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>-247435.4337257016</v>
+        <v>-1997.291766057096</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -964,7 +964,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>42078.77709494718</v>
+        <v>-2020.020294147966</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -972,7 +972,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>153805.9197667036</v>
+        <v>-1948.731695737526</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -980,7 +980,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>279737.4178199755</v>
+        <v>-1952.037018573134</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -988,7 +988,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>-466567.3486983348</v>
+        <v>-1880.039870115615</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -996,7 +996,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>-522364.3064474727</v>
+        <v>-1875.081761426459</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1004,7 +1004,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>556157.1192507776</v>
+        <v>-1907.631957430888</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1012,7 +1012,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>-12093.36097511337</v>
+        <v>-1853.281170119549</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1020,7 +1020,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>23910.0996156745</v>
+        <v>-1835.790387995673</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1028,7 +1028,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>73169.03677646219</v>
+        <v>-120536.6535508656</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1036,7 +1036,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>-180434.3065636301</v>
+        <v>-1069.16908048592</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1044,7 +1044,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>-36545.03002989897</v>
+        <v>-1037.378309504954</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1052,7 +1052,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>-94579.50172202638</v>
+        <v>-1006.000617172101</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1060,7 +1060,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>-144129.4033345473</v>
+        <v>-959.7256246177544</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1068,7 +1068,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>95754.04597226686</v>
+        <v>-961.165293637821</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1076,7 +1076,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>-69480.55998880061</v>
+        <v>-927.8541838848761</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1084,7 +1084,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>73921.55247476441</v>
+        <v>-936.8959503854447</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1092,7 +1092,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>469075.5756903166</v>
+        <v>-895.9969601476033</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1100,7 +1100,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>-455589.7485458328</v>
+        <v>-911.9707307866365</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1108,7 +1108,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>-18241.78002623086</v>
+        <v>-924.4015243295261</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1116,7 +1116,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>-29162.55853985969</v>
+        <v>-905.1183041758055</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1124,7 +1124,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>-7788.583107404444</v>
+        <v>-97405.6188670859</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1132,7 +1132,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>78383.95725593147</v>
+        <v>-576.2131538399767</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1140,7 +1140,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>-142574.8695779124</v>
+        <v>-587.9169370934774</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1148,7 +1148,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>649139.5021616736</v>
+        <v>-576.4997619579231</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1156,7 +1156,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>-205640.7461551565</v>
+        <v>-580.4754121272406</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1164,7 +1164,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>-334004.8897567698</v>
+        <v>-584.211346050738</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1172,7 +1172,7 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>-237347.6535559399</v>
+        <v>-549.2474733542732</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1180,7 +1180,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>95013.32994560619</v>
+        <v>-549.8961023201276</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1188,7 +1188,7 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>410408.3043647594</v>
+        <v>-564.1062702315463</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1196,7 +1196,7 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>-676863.4549802182</v>
+        <v>-552.3092859922812</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1204,7 +1204,7 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>-114410.1424990093</v>
+        <v>-571.077061912014</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1212,7 +1212,7 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>449119.1706241657</v>
+        <v>-564.2036018871468</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1220,7 +1220,7 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>344002.9968726381</v>
+        <v>-577.220006708626</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1228,7 +1228,7 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>8746.426761484599</v>
+        <v>-570.724020188372</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1236,7 +1236,7 @@
         <v>110</v>
       </c>
       <c r="B111">
-        <v>-91837.73013464085</v>
+        <v>-553.3339442735194</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1244,7 +1244,7 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>-227668.7916283504</v>
+        <v>-530.3967074245548</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1252,7 +1252,7 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>28658.06455683825</v>
+        <v>-537.0728868010428</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1260,7 +1260,7 @@
         <v>113</v>
       </c>
       <c r="B114">
-        <v>241591.3027008031</v>
+        <v>-550.1331633514874</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1268,7 +1268,7 @@
         <v>114</v>
       </c>
       <c r="B115">
-        <v>174273.8409437428</v>
+        <v>-545.2585385317417</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1276,7 +1276,7 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>-450402.3683358772</v>
+        <v>-519.8537324430229</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1284,7 +1284,7 @@
         <v>116</v>
       </c>
       <c r="B117">
-        <v>-14117.92245848203</v>
+        <v>-528.5157178316325</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1292,7 +1292,7 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>-153822.2261477093</v>
+        <v>-508.5178836755719</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1300,7 +1300,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>7594.156636816238</v>
+        <v>-498.959295779198</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1308,7 +1308,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>-256514.0239809672</v>
+        <v>-498.1610634008524</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1316,7 +1316,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>382502.0912904764</v>
+        <v>-111069.0481202427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>